<commit_message>
update table with t2t unique
</commit_message>
<xml_diff>
--- a/inst/extdata/table_excluderanges_and_gaps.xlsx
+++ b/inst/extdata/table_excluderanges_and_gaps.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,7 +360,7 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Object</t>
+          <t>Full ID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -397,7 +397,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ce10.Boyle.ce10-blacklist.v2.bed</t>
+          <t>ce10.Boyle.ce10-blacklist.v2.rds</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -430,7 +430,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ce10.Kundaje.ce10-blacklist.bed</t>
+          <t>ce10.Kundaje.ce10-blacklist.rds</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -463,7 +463,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ce11.Boyle.ce11-blacklist.v2.bed</t>
+          <t>ce11.Boyle.ce11-blacklist.v2.rds</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>danRer10.Domingues.blacklisted.bed</t>
+          <t>danRer10.Domingues.blacklisted.rds</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -529,7 +529,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>danRer10.Yang.Supplemental_Table_19.ChIP-seq_black_list_in_the_zebrafish_genome.bed</t>
+          <t>danRer10.Yang.Supplemental_Table_19.ChIP-seq_black_list_in_the_zebrafish_genome.rds</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -562,7 +562,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>dm3.Boyle.dm3-blacklist.v2.bed</t>
+          <t>dm3.Boyle.dm3-blacklist.v2.rds</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -595,7 +595,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>dm3.Kundaje.dm3-blacklist.bed</t>
+          <t>dm3.Kundaje.dm3-blacklist.rds</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -628,7 +628,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>dm6.Boyle.dm6-blacklist.v2.bed</t>
+          <t>dm6.Boyle.dm6-blacklist.v2.rds</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -661,7 +661,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>hg19.Bernstein.Mint_Blacklist_hg19.bed</t>
+          <t>hg19.Bernstein.Mint_Blacklist_hg19.rds</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -694,7 +694,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>hg19.Birney.wgEncodeDacMapabilityConsensusExcludable.bed</t>
+          <t>hg19.Birney.wgEncodeDacMapabilityConsensusExcludable.rds</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -727,7 +727,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>hg19.Boyle.hg19-blacklist.v2.bed</t>
+          <t>hg19.Boyle.hg19-blacklist.v2.rds</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -760,7 +760,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>hg19.Crawford.wgEncodeDukeMapabilityRegionsExcludable.bed</t>
+          <t>hg19.Crawford.wgEncodeDukeMapabilityRegionsExcludable.rds</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -793,7 +793,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>hg19.Lareau.hg19_peaks.narrowPeak.bed</t>
+          <t>hg19.Lareau.hg19_peaks.narrowPeak.rds</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -826,7 +826,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>hg19.Lareau.hg19.full.blacklist.bed</t>
+          <t>hg19.Lareau.hg19.full.blacklist.rds</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -859,7 +859,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>hg19.Wold.hg19mitoblack.bed</t>
+          <t>hg19.Wold.hg19mitoblack.rds</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -892,7 +892,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>hg19.Yeo.eCLIP_blacklistregions.hg19.bed</t>
+          <t>hg19.Yeo.eCLIP_blacklistregions.hg19.rds</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -925,7 +925,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>hg38.Bernstein.Mint_Blacklist_GRCh38.bed</t>
+          <t>hg38.Bernstein.Mint_Blacklist_GRCh38.rds</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -958,7 +958,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>hg38.Boyle.hg38-blacklist.v2.bed</t>
+          <t>hg38.Boyle.hg38-blacklist.v2.rds</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -991,7 +991,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>hg38.Kundaje.GRCh38_unified_blacklist.bed</t>
+          <t>hg38.Kundaje.GRCh38_unified_blacklist.rds</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1024,7 +1024,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>hg38.Kundaje.GRCh38.blacklist.bed</t>
+          <t>hg38.Kundaje.GRCh38.blacklist.rds</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1057,7 +1057,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>hg38.Lareau.hg19_peaks.narrowPeak.bed</t>
+          <t>hg38.Lareau.hg38_peaks.narrowPeak.rds</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1090,7 +1090,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>hg38.Lareau.hg38.full.blacklist.bed</t>
+          <t>hg38.Lareau.hg38.full.blacklist.rds</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1123,7 +1123,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>hg38.Reddy.wgEncodeDacMapabilityConsensusExcludable.hg38.bed</t>
+          <t>hg38.Reddy.wgEncodeDacMapabilityConsensusExcludable.hg38.rds</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1156,7 +1156,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>hg38.Wimberley.peakPass60Perc_sorted.bed</t>
+          <t>hg38.Wimberley.peakPass60Perc_sorted.rds</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1189,7 +1189,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>hg38.Wold.hg38mitoblack.bed</t>
+          <t>hg38.Wold.hg38mitoblack.rds</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1222,7 +1222,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>hg38.Yeo.eCLIP_blacklistregions.hg38liftover.bed.fixed.bed</t>
+          <t>hg38.Yeo.eCLIP_blacklistregions.hg38liftover.bed.fixed.rds</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1255,7 +1255,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>mm10.Boyle.mm10-blacklist.v2.bed</t>
+          <t>mm10.Boyle.mm10-blacklist.v2.rds</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1288,7 +1288,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>mm10.Hardison.blacklist.full.bed</t>
+          <t>mm10.Hardison.blacklist.full.rds</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1321,7 +1321,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>mm10.Hardison.psublacklist.mm10.bed</t>
+          <t>mm10.Hardison.psublacklist.mm10.rds</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1354,7 +1354,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>mm10.Kundaje.anshul.blacklist.mm10.bed</t>
+          <t>mm10.Kundaje.anshul.blacklist.mm10.rds</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1387,7 +1387,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>mm10.Kundaje.mm10.blacklist.bed</t>
+          <t>mm10.Kundaje.mm10.blacklist.rds</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1420,7 +1420,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>mm10.Lareau.mm10_peaks.narrowPeak.bed</t>
+          <t>mm10.Lareau.mm10_peaks.narrowPeak.rds</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1453,7 +1453,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>mm10.Lareau.mm10.full.blacklist.bed</t>
+          <t>mm10.Lareau.mm10.full.blacklist.rds</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1486,7 +1486,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>mm10.Wold.mm10mitoblack.bed</t>
+          <t>mm10.Wold.mm10mitoblack.rds</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1519,7 +1519,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>mm9.Lareau.mm9_peaks.narrowPeak.bed</t>
+          <t>mm9.Lareau.mm9_peaks.narrowPeak.rds</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1552,7 +1552,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>mm9.Lareau.mm9.full.blacklist.bed</t>
+          <t>mm9.Lareau.mm9.full.blacklist.rds</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1585,7 +1585,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>mm9.Wold.mm9mitoblack.bed</t>
+          <t>mm9.Wold.mm9mitoblack.rds</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1618,7 +1618,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>T2T.excluderanges.excludable.bed</t>
+          <t>T2T.excluderanges.excludable.rds</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1651,7 +1651,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>T2T.Lareau.chm13v2.0_peaks.narrowPeak.bed</t>
+          <t>T2T.Lareau.chm13v2.0_peaks.narrowPeak.rds</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1684,7 +1684,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>TAIR10.Klasfeld.arabidopsis_blacklist_20inputs.bed</t>
+          <t>TAIR10.Klasfeld.arabidopsis_blacklist_20inputs.rds</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1717,7 +1717,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>TAIR10.Klasfeld.arabidopsis_greenscreen_20inputs.bed</t>
+          <t>TAIR10.Klasfeld.arabidopsis_greenscreen_20inputs.rds</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1750,7 +1750,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>TAIR10.Wimberley.predicted_excluded_list_sorted_0.6.bed</t>
+          <t>TAIR10.Wimberley.predicted_excluded_list_sorted_0.6.rds</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2014,12 +2014,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>hg38.UCSC.centromere.rds</t>
+          <t>hg38.UCSC.centromere.bed</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>mm10</t>
+          <t>hg38</t>
         </is>
       </c>
       <c r="C51">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>10 : 3,390 : 30,000,000</t>
+          <t>11 : 3,391 : 30,000,001</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2569,6 +2569,39 @@
       <c r="G67" t="inlineStr">
         <is>
           <t>http://genome.ucsc.edu/cgi-bin/hgTables?db=mm10&amp;hgta_group=map&amp;hgta_track=gap&amp;hgta_table=gap&amp;hgta_doSchema=describe+table+schema</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>T2T.UCSC.hgUnique.hg38.bed</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>T2T</t>
+        </is>
+      </c>
+      <c r="C68">
+        <v>615</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2 : 15,829 : 29,694,330</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="F68">
+        <v>2022</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>https://hgdownload.soe.ucsc.edu/hubs/GCA/009/914/755/GCA_009914755.4/bbi/GCA_009914755.4_T2T-CHM13v2.0.hgUnique/hgUnique.hg38.bb</t>
         </is>
       </c>
     </row>

</xml_diff>